<commit_message>
count of schools, student teacher ratio by cluster and sector
</commit_message>
<xml_diff>
--- a/data/moe2018.xlsx
+++ b/data/moe2018.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Pre-U\BN_UBD\4. SM2302_Software\git_test\grp-the-r-ones\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181A72D5-2936-4080-B507-325D80E6A265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AE04E3C-A891-4012-B2A8-BB707B8C02FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="7" xr2:uid="{F8130892-C8BB-44EF-BFAE-F11D3EAC512E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{F8130892-C8BB-44EF-BFAE-F11D3EAC512E}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="65">
   <si>
     <t>2.1.2</t>
   </si>
@@ -236,10 +236,10 @@
     <t>Title</t>
   </si>
   <si>
-    <t>2.1.1 NUMBER OF SCHOOLS ACCORDING TO EDUCATION LEVEL BY DISTRICT</t>
-  </si>
-  <si>
     <t>2.1.3 ENROLMENT ACCORDING TO EDUCATION LEVEL BY DISTRICT</t>
+  </si>
+  <si>
+    <t>2.1.1 NUMBER OF TEACHERS ACCORDING TO EDUCATION LEVEL BY DISTRICT</t>
   </si>
 </sst>
 </file>
@@ -909,7 +909,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1318,7 +1318,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1330,7 +1330,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -1607,7 +1607,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
@@ -1858,7 +1858,7 @@
   <dimension ref="A1:E45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -3440,8 +3440,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAEF23CC-162B-4453-B485-DA402BB711D9}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3484,11 +3484,11 @@
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>53</v>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3498,11 +3498,11 @@
       <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>53</v>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3512,11 +3512,11 @@
       <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>53</v>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,11 +3526,11 @@
       <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>53</v>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -3710,8 +3710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA1F36E-5E5B-4961-A28F-B389D182D955}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -3754,11 +3754,11 @@
       <c r="B4" s="16" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D4" s="16" t="s">
-        <v>53</v>
+      <c r="C4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -3768,11 +3768,11 @@
       <c r="B5" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D5" s="16" t="s">
-        <v>53</v>
+      <c r="C5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -3782,11 +3782,11 @@
       <c r="B6" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>53</v>
+      <c r="C6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -3796,11 +3796,11 @@
       <c r="B7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>53</v>
+      <c r="C7" s="16">
+        <v>0</v>
+      </c>
+      <c r="D7" s="16">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>